<commit_message>
- Update cho nam 2020
</commit_message>
<xml_diff>
--- a/KE TOAN 2020/THUẾ_2020.xlsx
+++ b/KE TOAN 2020/THUẾ_2020.xlsx
@@ -11,7 +11,7 @@
     <sheet name="TNDN" sheetId="3" r:id="rId2"/>
     <sheet name="MÔN BÀI" sheetId="4" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="144525"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="30">
   <si>
     <t>KHAI THUẾ</t>
   </si>
@@ -108,6 +108,9 @@
   </si>
   <si>
     <t>THUẾ MÔN BÀI NĂM 2020</t>
+  </si>
+  <si>
+    <t>THUẾ MÔN BÀI NĂM 2021</t>
   </si>
 </sst>
 </file>
@@ -495,7 +498,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -506,7 +509,7 @@
   <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -542,7 +545,7 @@
       <c r="B2" s="4">
         <v>-4665390</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2" s="4">
         <v>589085</v>
       </c>
       <c r="D2" s="4">
@@ -751,7 +754,7 @@
         <v>9972886</v>
       </c>
       <c r="D15" s="5">
-        <f t="shared" si="3"/>
+        <f>SUM(D10:D14)</f>
         <v>-2288223</v>
       </c>
       <c r="E15" s="5"/>
@@ -793,53 +796,61 @@
       <c r="A19" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B19" s="4"/>
-      <c r="C19" s="4"/>
+      <c r="B19" s="4">
+        <v>4319651</v>
+      </c>
+      <c r="C19" s="4">
+        <v>4319651</v>
+      </c>
       <c r="D19" s="4">
-        <f t="shared" ref="D19:D22" si="4">B19-C19</f>
-        <v>0</v>
-      </c>
-      <c r="E19" s="6">
-        <v>43580.041851851624</v>
-      </c>
+        <f>B19-C19</f>
+        <v>0</v>
+      </c>
+      <c r="E19" s="6"/>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B20" s="4"/>
-      <c r="C20" s="4"/>
+      <c r="B20" s="4">
+        <v>3722955</v>
+      </c>
+      <c r="C20" s="4">
+        <v>3722955</v>
+      </c>
       <c r="D20" s="4">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="E20" s="6">
-        <v>43670.940648148302</v>
-      </c>
+        <f t="shared" ref="D19:D22" si="4">B20-C20</f>
+        <v>0</v>
+      </c>
+      <c r="E20" s="6"/>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B21" s="4"/>
-      <c r="C21" s="4"/>
+      <c r="B21" s="4">
+        <v>8075555</v>
+      </c>
+      <c r="C21" s="4">
+        <v>8075555</v>
+      </c>
       <c r="D21" s="4">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="E21" s="6">
-        <v>43765.962592592463</v>
-      </c>
+      <c r="E21" s="6"/>
     </row>
     <row r="22" spans="1:5">
       <c r="A22" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B22" s="4"/>
+      <c r="B22" s="4">
+        <v>3989945</v>
+      </c>
       <c r="C22" s="4"/>
       <c r="D22" s="4">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>3989945</v>
       </c>
       <c r="E22" s="1"/>
     </row>
@@ -849,15 +860,15 @@
       </c>
       <c r="B23" s="5">
         <f>SUM(B18:B22)</f>
-        <v>-2288223</v>
+        <v>17819883</v>
       </c>
       <c r="C23" s="5">
         <f t="shared" ref="C23:D23" si="5">SUM(C18:C22)</f>
-        <v>2966252</v>
+        <v>19084413</v>
       </c>
       <c r="D23" s="5">
         <f t="shared" si="5"/>
-        <v>-5254475</v>
+        <v>-1264530</v>
       </c>
       <c r="E23" s="5"/>
     </row>
@@ -872,7 +883,7 @@
   <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:E7"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1147,11 +1158,15 @@
       <c r="A19" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B19" s="4"/>
-      <c r="C19" s="4"/>
+      <c r="B19" s="4">
+        <v>7354211.6000000006</v>
+      </c>
+      <c r="C19" s="4">
+        <v>1470842</v>
+      </c>
       <c r="D19" s="4">
         <f t="shared" ref="D19:D22" si="4">B19-C19</f>
-        <v>0</v>
+        <v>5883369.6000000006</v>
       </c>
       <c r="E19" s="1"/>
     </row>
@@ -1159,11 +1174,15 @@
       <c r="A20" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B20" s="4"/>
-      <c r="C20" s="4"/>
+      <c r="B20" s="4">
+        <v>6684178.2000000002</v>
+      </c>
+      <c r="C20" s="4">
+        <v>5000000</v>
+      </c>
       <c r="D20" s="4">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>1684178.2000000002</v>
       </c>
       <c r="E20" s="1"/>
     </row>
@@ -1171,11 +1190,15 @@
       <c r="A21" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B21" s="4"/>
-      <c r="C21" s="4"/>
+      <c r="B21" s="4">
+        <v>14518739.085601091</v>
+      </c>
+      <c r="C21" s="4">
+        <v>12000000</v>
+      </c>
       <c r="D21" s="4">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>2518739.0856010914</v>
       </c>
       <c r="E21" s="1"/>
     </row>
@@ -1183,11 +1206,13 @@
       <c r="A22" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B22" s="4"/>
+      <c r="B22" s="4">
+        <v>7164720.5594954491</v>
+      </c>
       <c r="C22" s="4"/>
       <c r="D22" s="4">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>7164720.5594954491</v>
       </c>
       <c r="E22" s="1"/>
     </row>
@@ -1197,15 +1222,15 @@
       </c>
       <c r="B23" s="5">
         <f>SUM(B18:B22)</f>
-        <v>6374822.3762811683</v>
+        <v>42096671.82137771</v>
       </c>
       <c r="C23" s="5">
         <f t="shared" ref="C23:D23" si="5">SUM(C18:C22)</f>
-        <v>5319633</v>
+        <v>23790475</v>
       </c>
       <c r="D23" s="5">
         <f t="shared" si="5"/>
-        <v>1055189.3762811683</v>
+        <v>18306196.82137771</v>
       </c>
       <c r="E23" s="3"/>
     </row>
@@ -1217,10 +1242,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:E12"/>
+  <dimension ref="A2:E16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1385,6 +1410,57 @@
       </c>
       <c r="E12" s="3"/>
     </row>
+    <row r="14" spans="1:5">
+      <c r="A14" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B15" s="4">
+        <v>2000000</v>
+      </c>
+      <c r="C15" s="4">
+        <v>2000000</v>
+      </c>
+      <c r="D15" s="4">
+        <f>B15-C15</f>
+        <v>0</v>
+      </c>
+      <c r="E15" s="1"/>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B16" s="5">
+        <f>SUM(B15:B15)</f>
+        <v>2000000</v>
+      </c>
+      <c r="C16" s="5">
+        <f>SUM(C15:C15)</f>
+        <v>2000000</v>
+      </c>
+      <c r="D16" s="5">
+        <f>SUM(D15:D15)</f>
+        <v>0</v>
+      </c>
+      <c r="E16" s="3"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>